<commit_message>
upload astimate - TanLoc
</commit_message>
<xml_diff>
--- a/Task/M2M-005/M2M-005-estimate.xlsx
+++ b/Task/M2M-005/M2M-005-estimate.xlsx
@@ -71,7 +71,7 @@
     <t>F005_004</t>
   </si>
   <si>
-    <t>Detailed coding  of product functions</t>
+    <t>Fig bug</t>
   </si>
   <si>
     <t>F005_005</t>
@@ -1106,7 +1106,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="6" outlineLevelCol="3"/>
@@ -1136,11 +1136,11 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <f>C2/8</f>
-        <v>0.4375</v>
+        <f>C2/4</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1154,8 +1154,8 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <f>C3/8</f>
-        <v>0.125</v>
+        <f>C3/4</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1169,8 +1169,8 @@
         <v>1.5</v>
       </c>
       <c r="D4">
-        <f>C4/8</f>
-        <v>0.1875</v>
+        <f>C4/4</f>
+        <v>0.375</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1184,8 +1184,8 @@
         <v>1.5</v>
       </c>
       <c r="D5">
-        <f>C5/8</f>
-        <v>0.1875</v>
+        <f>C5/4</f>
+        <v>0.375</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1199,8 +1199,8 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <f>C6/8</f>
-        <v>0.125</v>
+        <f>C6/4</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="2:4">
@@ -1209,11 +1209,11 @@
       </c>
       <c r="C7" s="1">
         <f>SUM(C2:C6)</f>
-        <v>8.5</v>
-      </c>
-      <c r="D7" s="1">
-        <f>SUM(D2:D6)</f>
-        <v>1.0625</v>
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <f>C7/4</f>
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>